<commit_message>
Template project for ARDI board
</commit_message>
<xml_diff>
--- a/Boards/ARDI/Docs/Pinout.xlsx
+++ b/Boards/ARDI/Docs/Pinout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\RPCLib\Boards\ARDI\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Github\RPCLib\MIPS\Boards\ARDI\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C184ABB-44A9-42F9-A4DF-C97CB7D55E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E10DBF8-780A-406A-9742-885A5C3F9CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14730" yWindow="0" windowWidth="13755" windowHeight="9405" xr2:uid="{A5AD132A-4BD8-496E-BBC5-FCE4FC212F1D}"/>
+    <workbookView xWindow="-20610" yWindow="435" windowWidth="20730" windowHeight="11220" xr2:uid="{A5AD132A-4BD8-496E-BBC5-FCE4FC212F1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
   <si>
     <t>Pin</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>SW_SDA</t>
-  </si>
-  <si>
     <t>Digital Input</t>
   </si>
   <si>
@@ -198,15 +195,9 @@
     <t>RB2</t>
   </si>
   <si>
-    <t>I2C 2 SDA</t>
-  </si>
-  <si>
     <t>RB3</t>
   </si>
   <si>
-    <t>I2C 2 SCL</t>
-  </si>
-  <si>
     <t>RC0</t>
   </si>
   <si>
@@ -330,9 +321,6 @@
     <t>RB8</t>
   </si>
   <si>
-    <t>SW_SCL</t>
-  </si>
-  <si>
     <t>Connect to Cellular pin C104/RXD</t>
   </si>
   <si>
@@ -361,6 +349,24 @@
   </si>
   <si>
     <t>UART 3 RX</t>
+  </si>
+  <si>
+    <t>I2C1 SDA</t>
+  </si>
+  <si>
+    <t>I2C1 SCL</t>
+  </si>
+  <si>
+    <t>I2C2 SDA</t>
+  </si>
+  <si>
+    <t>I2C2 SCL</t>
+  </si>
+  <si>
+    <t>SENSOR_SCL</t>
+  </si>
+  <si>
+    <t>SENSOR_SDA</t>
   </si>
 </sst>
 </file>
@@ -745,17 +751,17 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -781,710 +787,710 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
       </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>9</v>
+        <v>102</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
       </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>101</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>100</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>86</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
+        <v>89</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>64</v>
+        <v>20</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>103</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1" xr:uid="{D91A35EC-B9E6-44E4-93FE-087862308308}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
-      <sortCondition ref="D1"/>
+      <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>